<commit_message>
final fitted distributions 3/12
</commit_message>
<xml_diff>
--- a/Data/qaly_input.xlsx
+++ b/Data/qaly_input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceguan/Dropbox/0_Stanford/Winter2020/HRP 263/Notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceguan/Dropbox/0_Stanford/Winter2020/HRP 263/Notebooks/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D1A7DE0-62A6-D140-9856-24988FC52634}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF6045D-F5E5-8F45-B95C-B65616F702AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="-20000" windowWidth="28040" windowHeight="17440" xr2:uid="{4F33316B-05AB-4748-B53C-5D439909DD2E}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,13 +436,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.73399999999999999</v>
+        <v>0.83</v>
       </c>
       <c r="C2">
-        <v>0.59799999999999998</v>
+        <v>0.77</v>
       </c>
       <c r="D2">
-        <v>0.871</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -450,13 +450,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.52</v>
+        <v>0.67</v>
       </c>
       <c r="C3">
-        <v>0.3</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D3">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -467,10 +467,10 @@
         <v>0.85</v>
       </c>
       <c r="C4">
-        <v>0.83</v>
+        <v>0.74</v>
       </c>
       <c r="D4">
-        <v>0.87</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -484,7 +484,7 @@
         <v>0.6</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>